<commit_message>
Files are complete so far for these. spectro_from_wav_audacity_match.py and spectro_from_wav_downsampling.py return similar peak magnitudes as fft_from_wav.py. The only difference is that there are different magnitudes -- will need to use the 1kHz tone and the STWINK within OnBoardMics project to determine a valid magnitude, and convert the magnitudes from the python files to what they would be expected in the OnBoardProject. spectro_from_wav_nfft.py does not give similar results to fft_from_wav.py but is useful because it somehow calculates the frequencies at each time stamp
</commit_message>
<xml_diff>
--- a/output_data.xlsx
+++ b/output_data.xlsx
@@ -393,82 +393,82 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>419</v>
+        <v>375</v>
       </c>
       <c r="B2">
-        <v>0.04478981526692708</v>
+        <v>426.3756408691406</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>355</v>
+        <v>187.5</v>
       </c>
       <c r="B3">
-        <v>0.04215080006917318</v>
+        <v>148.458251953125</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>390</v>
+        <v>3375</v>
       </c>
       <c r="B4">
-        <v>0.03496395619710287</v>
+        <v>132.2644958496094</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>1510</v>
+        <v>3703.125</v>
       </c>
       <c r="B5">
-        <v>0.02645222727457682</v>
+        <v>121.7497406005859</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>3083</v>
+        <v>843.75</v>
       </c>
       <c r="B6">
-        <v>0.02229311370849609</v>
+        <v>105.3359527587891</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>381</v>
+        <v>1500</v>
       </c>
       <c r="B7">
-        <v>0.02119811375935872</v>
+        <v>97.34624481201172</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>360</v>
+        <v>937.5</v>
       </c>
       <c r="B8">
-        <v>0.02086308034261068</v>
+        <v>91.82764434814453</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>1364</v>
+        <v>1218.75</v>
       </c>
       <c r="B9">
-        <v>0.01761422475179036</v>
+        <v>88.96601104736328</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>425</v>
+        <v>1406.25</v>
       </c>
       <c r="B10">
-        <v>0.01663838577270508</v>
+        <v>83.01222991943359</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>3366</v>
+        <v>562.5</v>
       </c>
       <c r="B11">
-        <v>0.01658476003011068</v>
+        <v>78.421142578125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new STM32 codes. First push for them, yet they are incomplete as they only process 21ms of data, and not the whole data at 21ms chunks
</commit_message>
<xml_diff>
--- a/output_data.xlsx
+++ b/output_data.xlsx
@@ -393,82 +393,82 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>375</v>
+        <v>562.5</v>
       </c>
       <c r="B2">
-        <v>426.3756408691406</v>
+        <v>1633.304321289062</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>187.5</v>
+        <v>1125</v>
       </c>
       <c r="B3">
-        <v>148.458251953125</v>
+        <v>47.20366668701172</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>3375</v>
+        <v>1687.5</v>
       </c>
       <c r="B4">
-        <v>132.2644958496094</v>
+        <v>29.50435256958008</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>3703.125</v>
+        <v>2718.75</v>
       </c>
       <c r="B5">
-        <v>121.7497406005859</v>
+        <v>24.51774406433105</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>843.75</v>
+        <v>2250</v>
       </c>
       <c r="B6">
-        <v>105.3359527587891</v>
+        <v>17.87451934814453</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>1500</v>
+        <v>3328.125</v>
       </c>
       <c r="B7">
-        <v>97.34624481201172</v>
+        <v>11.60765075683594</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>937.5</v>
+        <v>3000</v>
       </c>
       <c r="B8">
-        <v>91.82764434814453</v>
+        <v>9.267233848571777</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>1218.75</v>
+        <v>3562.5</v>
       </c>
       <c r="B9">
-        <v>88.96601104736328</v>
+        <v>9.189947128295898</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>1406.25</v>
+        <v>3890.625</v>
       </c>
       <c r="B10">
-        <v>83.01222991943359</v>
+        <v>9.049626350402832</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>562.5</v>
+        <v>3187.5</v>
       </c>
       <c r="B11">
-        <v>78.421142578125</v>
+        <v>8.95585823059082</v>
       </c>
     </row>
   </sheetData>

</xml_diff>